<commit_message>
added Menu, fixed ball getting stuck, Paddle Rotation and Screen Resolutions fixes
</commit_message>
<xml_diff>
--- a/TimeSheets/Time Log template_SEE.xlsx
+++ b/TimeSheets/Time Log template_SEE.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Wrote Overview for interation 1</t>
+  </si>
+  <si>
+    <t>7:00pm</t>
+  </si>
+  <si>
+    <t>8:00am</t>
+  </si>
+  <si>
+    <t>Created login, register buttons, modal and functionality</t>
   </si>
 </sst>
 </file>
@@ -556,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,12 +770,24 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="2">
+        <v>41954</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6">
+        <v>720</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>